<commit_message>
add new archives database , create database student and model database student
</commit_message>
<xml_diff>
--- a/Simulação_banco_escola.xlsx
+++ b/Simulação_banco_escola.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Table_student</t>
   </si>
@@ -78,7 +78,7 @@
     <t>nome</t>
   </si>
   <si>
-    <t xml:space="preserve">Andre Morales</t>
+    <t xml:space="preserve">André Morales</t>
   </si>
   <si>
     <t xml:space="preserve">Design Gráfico</t>
@@ -87,7 +87,7 @@
     <t xml:space="preserve">Eleandro Marcherino</t>
   </si>
   <si>
-    <t xml:space="preserve">Lógica de Programação</t>
+    <t xml:space="preserve">Pensamento Computacional</t>
   </si>
   <si>
     <t xml:space="preserve">NUMBER FOREING KEY (PROFILE)</t>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Table_classes</t>
+  </si>
+  <si>
+    <t>Id_order</t>
   </si>
   <si>
     <t>Id_teacher</t>
@@ -118,7 +121,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -182,13 +185,6 @@
       <name val="Calibri"/>
       <color theme="1" tint="0"/>
       <sz val="14.000000"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -280,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -335,7 +331,6 @@
     <xf fontId="7" fillId="10" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="10" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="3" fillId="9" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -858,7 +853,7 @@
     <col bestFit="1" customWidth="1" min="4" max="4" width="17.0859375"/>
     <col bestFit="1" customWidth="1" min="5" max="5" width="33.28125"/>
     <col bestFit="1" customWidth="1" min="6" max="6" width="45.28125"/>
-    <col bestFit="1" customWidth="1" min="7" max="7" width="29.00390625"/>
+    <col customWidth="1" min="7" max="7" width="31.140625"/>
     <col bestFit="1" customWidth="1" min="8" max="8" width="19.54296875"/>
   </cols>
   <sheetData>
@@ -1172,7 +1167,9 @@
       <c r="E15" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="22"/>
+      <c r="F15" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1182,20 +1179,22 @@
       <c r="M15" s="2"/>
     </row>
     <row r="16" ht="18.75">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="23" t="s">
-        <v>31</v>
+      <c r="B16" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="23">
+      <c r="D16" s="22">
         <v>1</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="22">
+        <v>1</v>
+      </c>
+      <c r="F16" s="22">
         <v>2</v>
       </c>
-      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1205,20 +1204,22 @@
       <c r="M16" s="2"/>
     </row>
     <row r="17" ht="18.75">
-      <c r="A17" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>32</v>
+      <c r="A17" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>33</v>
       </c>
       <c r="C17" s="17"/>
-      <c r="D17" s="23">
+      <c r="D17" s="22">
+        <v>2</v>
+      </c>
+      <c r="E17" s="22">
         <v>1</v>
       </c>
-      <c r="E17" s="23">
+      <c r="F17" s="22">
         <v>201</v>
       </c>
-      <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1228,16 +1229,18 @@
       <c r="M17" s="2"/>
     </row>
     <row r="18" ht="18.75">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="17"/>
-      <c r="D18" s="23">
+      <c r="D18" s="22">
+        <v>3</v>
+      </c>
+      <c r="E18" s="22">
         <v>1</v>
       </c>
-      <c r="E18" s="23">
+      <c r="F18" s="22">
         <v>1</v>
       </c>
-      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -1250,13 +1253,15 @@
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
-      <c r="D19" s="23">
+      <c r="D19" s="22">
+        <v>4</v>
+      </c>
+      <c r="E19" s="22">
         <v>2</v>
       </c>
-      <c r="E19" s="23">
+      <c r="F19" s="22">
         <v>1</v>
       </c>
-      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1269,13 +1274,15 @@
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
-      <c r="D20" s="23">
+      <c r="D20" s="22">
+        <v>5</v>
+      </c>
+      <c r="E20" s="22">
         <v>2</v>
       </c>
-      <c r="E20" s="23">
+      <c r="F20" s="22">
         <v>2</v>
       </c>
-      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1288,13 +1295,15 @@
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="17"/>
-      <c r="D21" s="23">
+      <c r="D21" s="22">
+        <v>6</v>
+      </c>
+      <c r="E21" s="22">
         <v>3</v>
       </c>
-      <c r="E21" s="23">
+      <c r="F21" s="22">
         <v>1</v>
       </c>
-      <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1307,13 +1316,15 @@
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="17"/>
-      <c r="D22" s="23">
+      <c r="D22" s="22">
+        <v>7</v>
+      </c>
+      <c r="E22" s="22">
         <v>3</v>
       </c>
-      <c r="E22" s="23">
+      <c r="F22" s="22">
         <v>201</v>
       </c>
-      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1326,13 +1337,15 @@
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="17"/>
-      <c r="D23" s="23">
+      <c r="D23" s="22">
+        <v>8</v>
+      </c>
+      <c r="E23" s="22">
         <v>3</v>
       </c>
-      <c r="E23" s="23">
+      <c r="F23" s="22">
         <v>2</v>
       </c>
-      <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>

</xml_diff>